<commit_message>
changed cabbage to be a green
</commit_message>
<xml_diff>
--- a/code/ProjectCode/Ingredients.xlsx
+++ b/code/ProjectCode/Ingredients.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmaneil/cs334/CS334-Final-Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmaneil/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E2F0EFC4-82D9-1F4A-950A-DAAD02A0BEC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F498DB82-E9A6-A94F-B721-FC8FA955EA3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="140" yWindow="480" windowWidth="28660" windowHeight="16120" xr2:uid="{13EE0B30-CE7D-4545-9524-AD5F66A30520}"/>
   </bookViews>
@@ -726,8 +726,8 @@
   <dimension ref="A1:H88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="141" zoomScaleNormal="190" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H72" sqref="H72"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A29" sqref="A29:XFD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -947,25 +947,25 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="B9" s="2">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9" t="s">
         <v>16</v>
@@ -973,36 +973,36 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2">
-        <v>4</v>
+        <v>0.25</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B11" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
         <v>38</v>
@@ -1011,7 +1011,7 @@
         <v>1</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -1025,16 +1025,16 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="2">
-        <v>0.25</v>
+        <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -1051,13 +1051,13 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B13" s="2">
         <v>0.25</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1077,13 +1077,13 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B14" s="2">
-        <v>4</v>
+        <v>0.25</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -1103,7 +1103,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="B15" s="2">
         <v>4</v>
@@ -1129,7 +1129,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="B16" s="2">
         <v>4</v>
@@ -1144,10 +1144,10 @@
         <v>0</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" t="s">
         <v>32</v>
@@ -1155,7 +1155,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" s="2">
         <v>4</v>
@@ -1164,7 +1164,7 @@
         <v>38</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -1173,7 +1173,7 @@
         <v>0</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" t="s">
         <v>32</v>
@@ -1181,16 +1181,16 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B18" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -1199,7 +1199,7 @@
         <v>0</v>
       </c>
       <c r="G18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H18" t="s">
         <v>32</v>
@@ -1207,13 +1207,13 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B19" s="2">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -1233,13 +1233,13 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B20" s="2">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="C20" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -1248,10 +1248,10 @@
         <v>0</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" t="s">
         <v>32</v>
@@ -1259,13 +1259,13 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="B21" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -1285,10 +1285,10 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="B22" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C22" t="s">
         <v>38</v>
@@ -1311,13 +1311,13 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B23" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -1337,13 +1337,13 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B24" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -1363,7 +1363,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="B25" s="2">
         <v>5</v>
@@ -1372,13 +1372,13 @@
         <v>38</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25">
         <v>0</v>
@@ -1389,7 +1389,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B26" s="2">
         <v>5</v>
@@ -1415,22 +1415,22 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="B27" s="2">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G27">
         <v>0</v>
@@ -1441,22 +1441,22 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="B28" s="2">
-        <v>0.125</v>
+        <v>0.5</v>
       </c>
       <c r="C28" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D28">
         <v>0</v>
       </c>
       <c r="E28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G28">
         <v>0</v>

</xml_diff>